<commit_message>
working on some tests
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobatjazi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobatjazi\Desktop\projects\file_validatiom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7167E69F-F467-4581-98EC-10B2362D1FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2324E89D-62E4-458E-AB59-C510985D7571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="12900" xr2:uid="{912F89F2-46CF-40F3-BDF0-487120830FA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{912F89F2-46CF-40F3-BDF0-487120830FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DrClinicHvDmgCase" sheetId="2" r:id="rId1"/>
@@ -927,7 +927,7 @@
   <dimension ref="A1:BB69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1180,7 @@
         <v>1076500</v>
       </c>
       <c r="J2" s="4">
-        <v>968850</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
implements SHARH and CLASS.COPY functionalities and temporarily removes label width
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobatjazi\Desktop\projects\file_validatiom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571DB9D0-A70E-4414-AC72-FAAC707F3301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDC28E-5550-4D3D-BA92-89CC793D8DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{912F89F2-46CF-40F3-BDF0-487120830FA3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="12900" xr2:uid="{912F89F2-46CF-40F3-BDF0-487120830FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="DrClinicHvDmgCase" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="139">
   <si>
     <t>ردیف</t>
   </si>
@@ -446,6 +446,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>نوموخوام</t>
+  </si>
+  <si>
+    <t>موخوام</t>
+  </si>
+  <si>
+    <t>شسمنیتشمنی</t>
   </si>
 </sst>
 </file>
@@ -455,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\ mmmm\ dddd\,\ dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +474,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -473,8 +481,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -506,33 +522,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,631 +872,631 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545F4537-52EC-4424-AE2A-1CB3EB25DA47}">
   <dimension ref="A1:BB69"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.25" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.25" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" style="16"/>
-    <col min="26" max="26" width="8.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24.25" style="17" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.25" style="17" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.25" style="16" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6" style="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="37.75" style="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.75" style="16" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.125" style="16" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.375" style="16" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.875" style="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8" style="16" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="9" style="9"/>
-    <col min="55" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="4.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" style="12"/>
+    <col min="26" max="26" width="8.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7" style="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" style="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="37.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21" style="12" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.375" style="12" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="9" style="5"/>
+    <col min="55" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:54" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AY1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="6" t="s">
+      <c r="AZ1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BA1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BB1" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12">
+    <row r="2" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
         <v>404706</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
-        <v>0</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12" t="s">
+      <c r="G2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="8">
         <v>15255621</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="12">
+      <c r="Q2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="8">
         <v>6728120</v>
       </c>
-      <c r="S2" s="12">
-        <v>0</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" s="12" t="s">
+      <c r="S2" s="8">
+        <v>0</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="14">
+      <c r="V2" s="8"/>
+      <c r="W2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="10">
         <v>107650</v>
       </c>
-      <c r="Z2" s="14">
+      <c r="Z2" s="10">
         <v>107650</v>
       </c>
-      <c r="AA2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="15">
+      <c r="AA2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="11">
         <v>45167.427083333336</v>
       </c>
-      <c r="AI2" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AJ2" s="15">
+      <c r="AI2" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AJ2" s="11">
         <v>45167.427083333336</v>
       </c>
-      <c r="AK2" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AL2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO2" s="12">
+      <c r="AK2" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AL2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO2" s="8">
         <v>6728118</v>
       </c>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="12"/>
-      <c r="AV2" s="12" t="s">
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
-      <c r="AY2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="12" t="s">
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BA2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB2" s="13" t="s">
+      <c r="BA2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB2" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+    <row r="3" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="8">
         <v>404706</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="14">
-        <v>1</v>
-      </c>
-      <c r="I3" s="14">
-        <v>1</v>
-      </c>
-      <c r="J3" s="14">
-        <v>0</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12" t="s">
+      <c r="G3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="10">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="8">
         <v>15255636</v>
       </c>
-      <c r="Q3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="12">
+      <c r="Q3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="8">
         <v>6728120</v>
       </c>
-      <c r="S3" s="12">
-        <v>0</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="12" t="s">
+      <c r="S3" s="8">
+        <v>0</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="14">
+      <c r="V3" s="8"/>
+      <c r="W3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="10">
         <v>78000</v>
       </c>
-      <c r="Z3" s="14">
+      <c r="Z3" s="10">
         <v>78000</v>
       </c>
-      <c r="AA3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="15">
+      <c r="AA3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="11">
         <v>45167.427777777775</v>
       </c>
-      <c r="AI3" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AJ3" s="15">
+      <c r="AI3" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AJ3" s="11">
         <v>45167.427777777775</v>
       </c>
-      <c r="AK3" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AL3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO3" s="12">
+      <c r="AK3" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AL3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO3" s="8">
         <v>6728118</v>
       </c>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="12" t="s">
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="12"/>
-      <c r="AY3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="12" t="s">
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BA3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB3" s="13" t="s">
+      <c r="BA3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB3" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+    <row r="4" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>404706</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12" t="s">
+      <c r="G4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="8">
         <v>15255659</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="12">
+      <c r="Q4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="8">
         <v>6728120</v>
       </c>
-      <c r="S4" s="12">
-        <v>0</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="12" t="s">
+      <c r="S4" s="8">
+        <v>0</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="14">
+      <c r="V4" s="8"/>
+      <c r="W4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="10">
         <v>160000</v>
       </c>
-      <c r="Z4" s="14">
+      <c r="Z4" s="10">
         <v>160000</v>
       </c>
-      <c r="AA4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="15">
+      <c r="AA4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="11">
         <v>45167.428472222222</v>
       </c>
-      <c r="AI4" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AJ4" s="15">
+      <c r="AI4" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AJ4" s="11">
         <v>45167.428472222222</v>
       </c>
-      <c r="AK4" s="12">
-        <v>41051010990</v>
-      </c>
-      <c r="AL4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO4" s="12">
+      <c r="AK4" s="8">
+        <v>41051010990</v>
+      </c>
+      <c r="AL4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO4" s="8">
         <v>6728118</v>
       </c>
-      <c r="AP4" s="12"/>
-      <c r="AQ4" s="12"/>
-      <c r="AR4" s="12"/>
-      <c r="AS4" s="12"/>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="12"/>
-      <c r="AV4" s="12" t="s">
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AW4" s="12"/>
-      <c r="AX4" s="12"/>
-      <c r="AY4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="12" t="s">
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BA4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB4" s="13" t="s">
+      <c r="BA4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB4" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1492,7 +1510,7 @@
       <c r="C5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1501,16 +1519,16 @@
       <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" s="14">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14">
-        <v>1</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="G5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
         <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1626,7 +1644,7 @@
       <c r="C6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1635,16 +1653,16 @@
       <c r="F6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="G6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1760,7 +1778,7 @@
       <c r="C7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1769,16 +1787,16 @@
       <c r="F7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7" s="14">
-        <v>1</v>
-      </c>
-      <c r="I7" s="14">
-        <v>1</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="G7" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10">
         <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1894,7 +1912,7 @@
       <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1903,16 +1921,16 @@
       <c r="F8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="G8" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
         <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -2028,7 +2046,7 @@
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -2037,16 +2055,16 @@
       <c r="F9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H9" s="14">
-        <v>1</v>
-      </c>
-      <c r="I9" s="14">
-        <v>1</v>
-      </c>
-      <c r="J9" s="14">
+      <c r="G9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10">
+        <v>1</v>
+      </c>
+      <c r="J9" s="10">
         <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -2162,7 +2180,7 @@
       <c r="C10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -2171,16 +2189,16 @@
       <c r="F10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="G10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="10">
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -2296,7 +2314,7 @@
       <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2305,16 +2323,16 @@
       <c r="F11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11" s="14">
+      <c r="G11" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1</v>
+      </c>
+      <c r="J11" s="10">
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -2430,7 +2448,7 @@
       <c r="C12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -2439,16 +2457,16 @@
       <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
-        <v>1</v>
-      </c>
-      <c r="J12" s="14">
+      <c r="G12" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
         <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
@@ -2564,7 +2582,7 @@
       <c r="C13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -2573,16 +2591,16 @@
       <c r="F13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H13" s="14">
-        <v>1</v>
-      </c>
-      <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="14">
+      <c r="G13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
         <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -2698,7 +2716,7 @@
       <c r="C14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -2707,16 +2725,16 @@
       <c r="F14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="14">
+      <c r="G14" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
         <v>0</v>
       </c>
       <c r="K14" s="1" t="s">
@@ -2832,7 +2850,7 @@
       <c r="C15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -2841,16 +2859,16 @@
       <c r="F15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="14">
-        <v>1</v>
-      </c>
-      <c r="I15" s="14">
-        <v>1</v>
-      </c>
-      <c r="J15" s="14">
+      <c r="G15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="10">
+        <v>1</v>
+      </c>
+      <c r="J15" s="10">
         <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
@@ -2966,7 +2984,7 @@
       <c r="C16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -2975,16 +2993,16 @@
       <c r="F16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" s="14">
-        <v>1</v>
-      </c>
-      <c r="I16" s="14">
-        <v>1</v>
-      </c>
-      <c r="J16" s="14">
+      <c r="G16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10">
         <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
@@ -3100,7 +3118,7 @@
       <c r="C17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -3109,16 +3127,16 @@
       <c r="F17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1</v>
-      </c>
-      <c r="I17" s="14">
-        <v>1</v>
-      </c>
-      <c r="J17" s="14">
+      <c r="G17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="10">
+        <v>1</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10">
         <v>0</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -3234,7 +3252,7 @@
       <c r="C18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -3243,16 +3261,16 @@
       <c r="F18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H18" s="14">
-        <v>1</v>
-      </c>
-      <c r="I18" s="14">
-        <v>1</v>
-      </c>
-      <c r="J18" s="14">
+      <c r="G18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1</v>
+      </c>
+      <c r="I18" s="10">
+        <v>1</v>
+      </c>
+      <c r="J18" s="10">
         <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -3368,7 +3386,7 @@
       <c r="C19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -3377,16 +3395,16 @@
       <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14">
-        <v>1</v>
-      </c>
-      <c r="J19" s="14">
+      <c r="G19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10">
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -3502,7 +3520,7 @@
       <c r="C20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -3511,16 +3529,16 @@
       <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H20" s="14">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14">
-        <v>1</v>
-      </c>
-      <c r="J20" s="14">
+      <c r="G20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10">
         <v>0</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3636,7 +3654,7 @@
       <c r="C21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -3645,16 +3663,16 @@
       <c r="F21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H21" s="14">
-        <v>1</v>
-      </c>
-      <c r="I21" s="14">
-        <v>1</v>
-      </c>
-      <c r="J21" s="14">
+      <c r="G21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+      <c r="J21" s="10">
         <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -3770,7 +3788,7 @@
       <c r="C22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -3779,16 +3797,16 @@
       <c r="F22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H22" s="14">
-        <v>1</v>
-      </c>
-      <c r="I22" s="14">
-        <v>1</v>
-      </c>
-      <c r="J22" s="14">
+      <c r="G22" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="10">
         <v>0</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -3904,7 +3922,7 @@
       <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -3913,16 +3931,16 @@
       <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H23" s="14">
-        <v>1</v>
-      </c>
-      <c r="I23" s="14">
-        <v>1</v>
-      </c>
-      <c r="J23" s="14">
+      <c r="G23" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1</v>
+      </c>
+      <c r="I23" s="10">
+        <v>1</v>
+      </c>
+      <c r="J23" s="10">
         <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
@@ -4038,7 +4056,7 @@
       <c r="C24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -4047,16 +4065,16 @@
       <c r="F24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H24" s="14">
-        <v>1</v>
-      </c>
-      <c r="I24" s="14">
-        <v>1</v>
-      </c>
-      <c r="J24" s="14">
+      <c r="G24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="10">
+        <v>1</v>
+      </c>
+      <c r="J24" s="10">
         <v>0</v>
       </c>
       <c r="K24" s="1" t="s">
@@ -4172,7 +4190,7 @@
       <c r="C25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -4181,16 +4199,16 @@
       <c r="F25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" s="14">
-        <v>1</v>
-      </c>
-      <c r="I25" s="14">
-        <v>1</v>
-      </c>
-      <c r="J25" s="14">
+      <c r="G25" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="10">
+        <v>1</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
+      <c r="J25" s="10">
         <v>0</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -4306,7 +4324,7 @@
       <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -4315,16 +4333,16 @@
       <c r="F26" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H26" s="14">
-        <v>1</v>
-      </c>
-      <c r="I26" s="14">
-        <v>1</v>
-      </c>
-      <c r="J26" s="14">
+      <c r="G26" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H26" s="10">
+        <v>1</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1</v>
+      </c>
+      <c r="J26" s="10">
         <v>0</v>
       </c>
       <c r="K26" s="1" t="s">
@@ -4440,7 +4458,7 @@
       <c r="C27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -4449,16 +4467,16 @@
       <c r="F27" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="14">
-        <v>1</v>
-      </c>
-      <c r="I27" s="14">
-        <v>1</v>
-      </c>
-      <c r="J27" s="14">
+      <c r="G27" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10">
         <v>0</v>
       </c>
       <c r="K27" s="1" t="s">
@@ -4574,7 +4592,7 @@
       <c r="C28" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -4583,16 +4601,16 @@
       <c r="F28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H28" s="14">
-        <v>1</v>
-      </c>
-      <c r="I28" s="14">
-        <v>1</v>
-      </c>
-      <c r="J28" s="14">
+      <c r="G28" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="10">
+        <v>1</v>
+      </c>
+      <c r="I28" s="10">
+        <v>1</v>
+      </c>
+      <c r="J28" s="10">
         <v>0</v>
       </c>
       <c r="K28" s="1" t="s">
@@ -4708,7 +4726,7 @@
       <c r="C29" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -4717,16 +4735,16 @@
       <c r="F29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H29" s="14">
-        <v>1</v>
-      </c>
-      <c r="I29" s="14">
-        <v>1</v>
-      </c>
-      <c r="J29" s="14">
+      <c r="G29" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1</v>
+      </c>
+      <c r="J29" s="10">
         <v>0</v>
       </c>
       <c r="K29" s="1" t="s">
@@ -4842,7 +4860,7 @@
       <c r="C30" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -4851,16 +4869,16 @@
       <c r="F30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H30" s="14">
-        <v>1</v>
-      </c>
-      <c r="I30" s="14">
-        <v>1</v>
-      </c>
-      <c r="J30" s="14">
+      <c r="G30" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>1</v>
+      </c>
+      <c r="J30" s="10">
         <v>0</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -4976,7 +4994,7 @@
       <c r="C31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -4985,16 +5003,16 @@
       <c r="F31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H31" s="14">
-        <v>1</v>
-      </c>
-      <c r="I31" s="14">
-        <v>1</v>
-      </c>
-      <c r="J31" s="14">
+      <c r="G31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+      <c r="I31" s="10">
+        <v>1</v>
+      </c>
+      <c r="J31" s="10">
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -5110,7 +5128,7 @@
       <c r="C32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -5119,16 +5137,16 @@
       <c r="F32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H32" s="14">
-        <v>1</v>
-      </c>
-      <c r="I32" s="14">
-        <v>1</v>
-      </c>
-      <c r="J32" s="14">
+      <c r="G32" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
+      <c r="I32" s="10">
+        <v>1</v>
+      </c>
+      <c r="J32" s="10">
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
@@ -5244,7 +5262,7 @@
       <c r="C33" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -5253,16 +5271,16 @@
       <c r="F33" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H33" s="14">
-        <v>1</v>
-      </c>
-      <c r="I33" s="14">
-        <v>1</v>
-      </c>
-      <c r="J33" s="14">
+      <c r="G33" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+      <c r="I33" s="10">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10">
         <v>0</v>
       </c>
       <c r="K33" s="1" t="s">
@@ -5378,7 +5396,7 @@
       <c r="C34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -5387,16 +5405,16 @@
       <c r="F34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H34" s="14">
-        <v>1</v>
-      </c>
-      <c r="I34" s="14">
-        <v>1</v>
-      </c>
-      <c r="J34" s="14">
+      <c r="G34" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+      <c r="I34" s="10">
+        <v>1</v>
+      </c>
+      <c r="J34" s="10">
         <v>0</v>
       </c>
       <c r="K34" s="1" t="s">
@@ -5512,7 +5530,7 @@
       <c r="C35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -5521,16 +5539,16 @@
       <c r="F35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H35" s="14">
-        <v>1</v>
-      </c>
-      <c r="I35" s="14">
-        <v>1</v>
-      </c>
-      <c r="J35" s="14">
+      <c r="G35" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+      <c r="I35" s="10">
+        <v>1</v>
+      </c>
+      <c r="J35" s="10">
         <v>0</v>
       </c>
       <c r="K35" s="1" t="s">
@@ -5646,7 +5664,7 @@
       <c r="C36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -5655,16 +5673,16 @@
       <c r="F36" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H36" s="14">
-        <v>1</v>
-      </c>
-      <c r="I36" s="14">
-        <v>1</v>
-      </c>
-      <c r="J36" s="14">
+      <c r="G36" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10">
+        <v>1</v>
+      </c>
+      <c r="J36" s="10">
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
@@ -5780,7 +5798,7 @@
       <c r="C37" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -5789,16 +5807,16 @@
       <c r="F37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H37" s="14">
-        <v>1</v>
-      </c>
-      <c r="I37" s="14">
-        <v>1</v>
-      </c>
-      <c r="J37" s="14">
+      <c r="G37" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37" s="10">
+        <v>1</v>
+      </c>
+      <c r="J37" s="10">
         <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
@@ -5914,7 +5932,7 @@
       <c r="C38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -5923,16 +5941,16 @@
       <c r="F38" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G38" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H38" s="14">
-        <v>1</v>
-      </c>
-      <c r="I38" s="14">
-        <v>1</v>
-      </c>
-      <c r="J38" s="14">
+      <c r="G38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+      <c r="I38" s="10">
+        <v>1</v>
+      </c>
+      <c r="J38" s="10">
         <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
@@ -6048,7 +6066,7 @@
       <c r="C39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -6057,16 +6075,16 @@
       <c r="F39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H39" s="14">
-        <v>1</v>
-      </c>
-      <c r="I39" s="14">
-        <v>1</v>
-      </c>
-      <c r="J39" s="14">
+      <c r="G39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39" s="10">
+        <v>1</v>
+      </c>
+      <c r="J39" s="10">
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
@@ -6182,7 +6200,7 @@
       <c r="C40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -6191,16 +6209,16 @@
       <c r="F40" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H40" s="14">
-        <v>1</v>
-      </c>
-      <c r="I40" s="14">
-        <v>1</v>
-      </c>
-      <c r="J40" s="14">
+      <c r="G40" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" s="10">
+        <v>1</v>
+      </c>
+      <c r="I40" s="10">
+        <v>1</v>
+      </c>
+      <c r="J40" s="10">
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
@@ -6316,7 +6334,7 @@
       <c r="C41" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -6325,16 +6343,16 @@
       <c r="F41" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G41" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H41" s="14">
-        <v>1</v>
-      </c>
-      <c r="I41" s="14">
-        <v>1</v>
-      </c>
-      <c r="J41" s="14">
+      <c r="G41" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H41" s="10">
+        <v>1</v>
+      </c>
+      <c r="I41" s="10">
+        <v>1</v>
+      </c>
+      <c r="J41" s="10">
         <v>0</v>
       </c>
       <c r="K41" s="1" t="s">
@@ -6450,7 +6468,7 @@
       <c r="C42" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -6459,16 +6477,16 @@
       <c r="F42" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H42" s="14">
-        <v>1</v>
-      </c>
-      <c r="I42" s="14">
-        <v>1</v>
-      </c>
-      <c r="J42" s="14">
+      <c r="G42" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" s="10">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10">
+        <v>1</v>
+      </c>
+      <c r="J42" s="10">
         <v>0</v>
       </c>
       <c r="K42" s="1" t="s">
@@ -6584,7 +6602,7 @@
       <c r="C43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -6593,16 +6611,16 @@
       <c r="F43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G43" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H43" s="14">
-        <v>1</v>
-      </c>
-      <c r="I43" s="14">
-        <v>1</v>
-      </c>
-      <c r="J43" s="14">
+      <c r="G43" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H43" s="10">
+        <v>1</v>
+      </c>
+      <c r="I43" s="10">
+        <v>1</v>
+      </c>
+      <c r="J43" s="10">
         <v>0</v>
       </c>
       <c r="K43" s="1" t="s">
@@ -6718,7 +6736,7 @@
       <c r="C44" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -6727,16 +6745,16 @@
       <c r="F44" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G44" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H44" s="14">
-        <v>1</v>
-      </c>
-      <c r="I44" s="14">
-        <v>1</v>
-      </c>
-      <c r="J44" s="14">
+      <c r="G44" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44" s="10">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10">
+        <v>1</v>
+      </c>
+      <c r="J44" s="10">
         <v>0</v>
       </c>
       <c r="K44" s="1" t="s">
@@ -6852,7 +6870,7 @@
       <c r="C45" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -6861,16 +6879,16 @@
       <c r="F45" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G45" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H45" s="14">
-        <v>1</v>
-      </c>
-      <c r="I45" s="14">
-        <v>1</v>
-      </c>
-      <c r="J45" s="14">
+      <c r="G45" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H45" s="10">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10">
+        <v>1</v>
+      </c>
+      <c r="J45" s="10">
         <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
@@ -6986,7 +7004,7 @@
       <c r="C46" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -6995,16 +7013,16 @@
       <c r="F46" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G46" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H46" s="14">
-        <v>1</v>
-      </c>
-      <c r="I46" s="14">
-        <v>1</v>
-      </c>
-      <c r="J46" s="14">
+      <c r="G46" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10">
+        <v>1</v>
+      </c>
+      <c r="J46" s="10">
         <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
@@ -7120,7 +7138,7 @@
       <c r="C47" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -7129,16 +7147,16 @@
       <c r="F47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G47" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H47" s="14">
-        <v>1</v>
-      </c>
-      <c r="I47" s="14">
-        <v>1</v>
-      </c>
-      <c r="J47" s="14">
+      <c r="G47" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H47" s="10">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10">
+        <v>1</v>
+      </c>
+      <c r="J47" s="10">
         <v>0</v>
       </c>
       <c r="K47" s="1" t="s">
@@ -7254,7 +7272,7 @@
       <c r="C48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -7263,16 +7281,16 @@
       <c r="F48" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G48" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H48" s="14">
-        <v>1</v>
-      </c>
-      <c r="I48" s="14">
-        <v>1</v>
-      </c>
-      <c r="J48" s="14">
+      <c r="G48" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H48" s="10">
+        <v>1</v>
+      </c>
+      <c r="I48" s="10">
+        <v>1</v>
+      </c>
+      <c r="J48" s="10">
         <v>0</v>
       </c>
       <c r="K48" s="1" t="s">
@@ -7388,7 +7406,7 @@
       <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -7397,16 +7415,16 @@
       <c r="F49" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G49" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H49" s="14">
-        <v>1</v>
-      </c>
-      <c r="I49" s="14">
-        <v>1</v>
-      </c>
-      <c r="J49" s="14">
+      <c r="G49" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" s="10">
+        <v>1</v>
+      </c>
+      <c r="I49" s="10">
+        <v>1</v>
+      </c>
+      <c r="J49" s="10">
         <v>0</v>
       </c>
       <c r="K49" s="1" t="s">
@@ -7522,7 +7540,7 @@
       <c r="C50" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -7531,16 +7549,16 @@
       <c r="F50" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G50" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H50" s="14">
-        <v>1</v>
-      </c>
-      <c r="I50" s="14">
-        <v>1</v>
-      </c>
-      <c r="J50" s="14">
+      <c r="G50" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+      <c r="I50" s="10">
+        <v>1</v>
+      </c>
+      <c r="J50" s="10">
         <v>0</v>
       </c>
       <c r="K50" s="1" t="s">
@@ -7656,7 +7674,7 @@
       <c r="C51" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -7665,16 +7683,16 @@
       <c r="F51" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G51" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H51" s="14">
-        <v>1</v>
-      </c>
-      <c r="I51" s="14">
-        <v>1</v>
-      </c>
-      <c r="J51" s="14">
+      <c r="G51" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H51" s="10">
+        <v>1</v>
+      </c>
+      <c r="I51" s="10">
+        <v>1</v>
+      </c>
+      <c r="J51" s="10">
         <v>0</v>
       </c>
       <c r="K51" s="1" t="s">
@@ -7790,7 +7808,7 @@
       <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -7799,16 +7817,16 @@
       <c r="F52" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G52" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H52" s="14">
-        <v>1</v>
-      </c>
-      <c r="I52" s="14">
-        <v>1</v>
-      </c>
-      <c r="J52" s="14">
+      <c r="G52" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52" s="10">
+        <v>1</v>
+      </c>
+      <c r="I52" s="10">
+        <v>1</v>
+      </c>
+      <c r="J52" s="10">
         <v>0</v>
       </c>
       <c r="K52" s="1" t="s">
@@ -7924,7 +7942,7 @@
       <c r="C53" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -7933,16 +7951,16 @@
       <c r="F53" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H53" s="14">
-        <v>1</v>
-      </c>
-      <c r="I53" s="14">
-        <v>1</v>
-      </c>
-      <c r="J53" s="14">
+      <c r="G53" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H53" s="10">
+        <v>1</v>
+      </c>
+      <c r="I53" s="10">
+        <v>1</v>
+      </c>
+      <c r="J53" s="10">
         <v>0</v>
       </c>
       <c r="K53" s="1" t="s">
@@ -8058,7 +8076,7 @@
       <c r="C54" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -8067,16 +8085,16 @@
       <c r="F54" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G54" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H54" s="14">
-        <v>1</v>
-      </c>
-      <c r="I54" s="14">
-        <v>1</v>
-      </c>
-      <c r="J54" s="14">
+      <c r="G54" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H54" s="10">
+        <v>1</v>
+      </c>
+      <c r="I54" s="10">
+        <v>1</v>
+      </c>
+      <c r="J54" s="10">
         <v>0</v>
       </c>
       <c r="K54" s="1" t="s">
@@ -8192,7 +8210,7 @@
       <c r="C55" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -8201,16 +8219,16 @@
       <c r="F55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G55" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H55" s="14">
-        <v>1</v>
-      </c>
-      <c r="I55" s="14">
-        <v>1</v>
-      </c>
-      <c r="J55" s="14">
+      <c r="G55" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+      <c r="I55" s="10">
+        <v>1</v>
+      </c>
+      <c r="J55" s="10">
         <v>0</v>
       </c>
       <c r="K55" s="1" t="s">
@@ -8326,7 +8344,7 @@
       <c r="C56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -8335,16 +8353,16 @@
       <c r="F56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G56" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H56" s="14">
-        <v>1</v>
-      </c>
-      <c r="I56" s="14">
-        <v>1</v>
-      </c>
-      <c r="J56" s="14">
+      <c r="G56" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H56" s="10">
+        <v>1</v>
+      </c>
+      <c r="I56" s="10">
+        <v>1</v>
+      </c>
+      <c r="J56" s="10">
         <v>0</v>
       </c>
       <c r="K56" s="1" t="s">
@@ -8460,7 +8478,7 @@
       <c r="C57" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -8469,16 +8487,16 @@
       <c r="F57" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G57" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H57" s="14">
-        <v>1</v>
-      </c>
-      <c r="I57" s="14">
-        <v>1</v>
-      </c>
-      <c r="J57" s="14">
+      <c r="G57" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H57" s="10">
+        <v>1</v>
+      </c>
+      <c r="I57" s="10">
+        <v>1</v>
+      </c>
+      <c r="J57" s="10">
         <v>0</v>
       </c>
       <c r="K57" s="1" t="s">
@@ -8594,7 +8612,7 @@
       <c r="C58" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -8603,16 +8621,16 @@
       <c r="F58" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G58" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H58" s="14">
-        <v>1</v>
-      </c>
-      <c r="I58" s="14">
-        <v>1</v>
-      </c>
-      <c r="J58" s="14">
+      <c r="G58" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" s="10">
+        <v>1</v>
+      </c>
+      <c r="I58" s="10">
+        <v>1</v>
+      </c>
+      <c r="J58" s="10">
         <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
@@ -8728,7 +8746,7 @@
       <c r="C59" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -8737,16 +8755,16 @@
       <c r="F59" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G59" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H59" s="14">
-        <v>1</v>
-      </c>
-      <c r="I59" s="14">
-        <v>1</v>
-      </c>
-      <c r="J59" s="14">
+      <c r="G59" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H59" s="10">
+        <v>1</v>
+      </c>
+      <c r="I59" s="10">
+        <v>1</v>
+      </c>
+      <c r="J59" s="10">
         <v>0</v>
       </c>
       <c r="K59" s="1" t="s">
@@ -8862,7 +8880,7 @@
       <c r="C60" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -8871,16 +8889,16 @@
       <c r="F60" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G60" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H60" s="14">
-        <v>1</v>
-      </c>
-      <c r="I60" s="14">
-        <v>1</v>
-      </c>
-      <c r="J60" s="14">
+      <c r="G60" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H60" s="10">
+        <v>1</v>
+      </c>
+      <c r="I60" s="10">
+        <v>1</v>
+      </c>
+      <c r="J60" s="10">
         <v>0</v>
       </c>
       <c r="K60" s="1" t="s">
@@ -8996,7 +9014,7 @@
       <c r="C61" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -9005,16 +9023,16 @@
       <c r="F61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G61" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H61" s="14">
-        <v>1</v>
-      </c>
-      <c r="I61" s="14">
-        <v>1</v>
-      </c>
-      <c r="J61" s="14">
+      <c r="G61" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H61" s="10">
+        <v>1</v>
+      </c>
+      <c r="I61" s="10">
+        <v>1</v>
+      </c>
+      <c r="J61" s="10">
         <v>0</v>
       </c>
       <c r="K61" s="1" t="s">
@@ -9130,7 +9148,7 @@
       <c r="C62" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -9139,16 +9157,16 @@
       <c r="F62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G62" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H62" s="14">
-        <v>1</v>
-      </c>
-      <c r="I62" s="14">
-        <v>1</v>
-      </c>
-      <c r="J62" s="14">
+      <c r="G62" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H62" s="10">
+        <v>1</v>
+      </c>
+      <c r="I62" s="10">
+        <v>1</v>
+      </c>
+      <c r="J62" s="10">
         <v>0</v>
       </c>
       <c r="K62" s="1" t="s">
@@ -9264,7 +9282,7 @@
       <c r="C63" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -9273,16 +9291,16 @@
       <c r="F63" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G63" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H63" s="14">
-        <v>1</v>
-      </c>
-      <c r="I63" s="14">
-        <v>1</v>
-      </c>
-      <c r="J63" s="14">
+      <c r="G63" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H63" s="10">
+        <v>1</v>
+      </c>
+      <c r="I63" s="10">
+        <v>1</v>
+      </c>
+      <c r="J63" s="10">
         <v>0</v>
       </c>
       <c r="K63" s="1" t="s">
@@ -9398,7 +9416,7 @@
       <c r="C64" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E64" s="2" t="s">
@@ -9407,16 +9425,16 @@
       <c r="F64" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G64" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H64" s="14">
-        <v>1</v>
-      </c>
-      <c r="I64" s="14">
-        <v>1</v>
-      </c>
-      <c r="J64" s="14">
+      <c r="G64" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H64" s="10">
+        <v>1</v>
+      </c>
+      <c r="I64" s="10">
+        <v>1</v>
+      </c>
+      <c r="J64" s="10">
         <v>0</v>
       </c>
       <c r="K64" s="1" t="s">
@@ -9532,7 +9550,7 @@
       <c r="C65" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -9541,16 +9559,16 @@
       <c r="F65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G65" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H65" s="14">
-        <v>1</v>
-      </c>
-      <c r="I65" s="14">
-        <v>1</v>
-      </c>
-      <c r="J65" s="14">
+      <c r="G65" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65" s="10">
+        <v>1</v>
+      </c>
+      <c r="I65" s="10">
+        <v>1</v>
+      </c>
+      <c r="J65" s="10">
         <v>0</v>
       </c>
       <c r="K65" s="1" t="s">
@@ -9666,7 +9684,7 @@
       <c r="C66" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D66" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E66" s="2" t="s">
@@ -9675,16 +9693,16 @@
       <c r="F66" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G66" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H66" s="14">
-        <v>1</v>
-      </c>
-      <c r="I66" s="14">
-        <v>1</v>
-      </c>
-      <c r="J66" s="14">
+      <c r="G66" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H66" s="10">
+        <v>1</v>
+      </c>
+      <c r="I66" s="10">
+        <v>1</v>
+      </c>
+      <c r="J66" s="10">
         <v>0</v>
       </c>
       <c r="K66" s="1" t="s">
@@ -9800,7 +9818,7 @@
       <c r="C67" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -9809,16 +9827,16 @@
       <c r="F67" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H67" s="14">
-        <v>1</v>
-      </c>
-      <c r="I67" s="14">
-        <v>1</v>
-      </c>
-      <c r="J67" s="14">
+      <c r="G67" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H67" s="10">
+        <v>1</v>
+      </c>
+      <c r="I67" s="10">
+        <v>1</v>
+      </c>
+      <c r="J67" s="10">
         <v>0</v>
       </c>
       <c r="K67" s="1" t="s">
@@ -9934,7 +9952,7 @@
       <c r="C68" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="D68" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -9943,16 +9961,16 @@
       <c r="F68" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G68" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H68" s="14">
-        <v>1</v>
-      </c>
-      <c r="I68" s="14">
-        <v>1</v>
-      </c>
-      <c r="J68" s="14">
+      <c r="G68" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H68" s="10">
+        <v>1</v>
+      </c>
+      <c r="I68" s="10">
+        <v>1</v>
+      </c>
+      <c r="J68" s="10">
         <v>0</v>
       </c>
       <c r="K68" s="1" t="s">
@@ -10068,7 +10086,7 @@
       <c r="C69" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -10077,16 +10095,16 @@
       <c r="F69" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G69" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H69" s="14">
-        <v>1</v>
-      </c>
-      <c r="I69" s="14">
-        <v>1</v>
-      </c>
-      <c r="J69" s="14">
+      <c r="G69" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H69" s="10">
+        <v>1</v>
+      </c>
+      <c r="I69" s="10">
+        <v>1</v>
+      </c>
+      <c r="J69" s="10">
         <v>0</v>
       </c>
       <c r="K69" s="1" t="s">

</xml_diff>